<commit_message>
write_ts_xlsx now creates nicely formatted Excel files.
</commit_message>
<xml_diff>
--- a/examples/write_ts/test1.xlsx
+++ b/examples/write_ts/test1.xlsx
@@ -14,7 +14,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>names</t>
+    <t>name</t>
   </si>
   <si>
     <t>2010Q2</t>
@@ -69,8 +69,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
@@ -79,21 +82,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView workbookViewId="0" tabSelected="true">
+      <pane xSplit="1.0" ySplit="1.0" state="frozen" topLeftCell="B2" activePane="bottomRight"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="6.07421875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="8.18359375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="8.18359375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="8.18359375" customWidth="true" bestFit="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="1">
         <v>3</v>
       </c>
     </row>

</xml_diff>